<commit_message>
move SkillAttachStatus/SkillDetachStatus to Cfg_Skill
</commit_message>
<xml_diff>
--- a/server-res/excel/Cfg_Skill.xlsx
+++ b/server-res/excel/Cfg_Skill.xlsx
@@ -160,7 +160,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="90">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -416,6 +416,65 @@
   </si>
   <si>
     <t>调试</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>attach_status</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>detach_status</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>#memo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>给目标增加1个持续扣血的状态, 每3秒造成2点伤害, 持续30秒</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>血量上限增加50</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">message SkillAttachStatus
+{
+ uint32 typeid = 1;//BUUF类型ID    
+ uint32 lev  = 2;//BUUF等级
+ uint32 power = 3;//BUFF数值
+ uint32 secs = 4;//N秒1次
+ uint32 times = 5;//持续几次
+}
+</t>
+  </si>
+  <si>
+    <t>message SkillDetachStatus
+{
+ uint32 id   = 1;//状态编号  
+ uint32 type = 2;//状态类型
+ uint32 flag = 3;//状态掩码
+};</t>
+  </si>
+  <si>
+    <t>[{"type:2, "flag":2},{"flag":1}]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[{"id":5 , "lev":1 ,"power":2 ,"secs":3 ,"times":10 }]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[{ "id":1 , "lev":1 ,"power": ,"secs":60 ,"times":1 }]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[{"id":32}]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[{"type:1, "flag":3}]</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -423,7 +482,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -453,6 +512,21 @@
       <family val="3"/>
       <charset val="134"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -474,12 +548,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -784,43 +872,53 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AH16"/>
+  <dimension ref="A1:AL16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <pane xSplit="1" topLeftCell="AJ1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AJ8" sqref="AJ8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.75" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.75" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.875" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="11.125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.25" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.5" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="10.5" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="16.125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="5.5" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="10.5" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="12.75" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="17.25" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="35.875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.125" bestFit="1" customWidth="1"/>
-    <col min="22" max="23" width="11.125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="13" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="24" max="25" width="9.5" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="13.875" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="13" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="9" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="13" bestFit="1" customWidth="1"/>
+    <col min="27" max="28" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.75" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="13.875" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="58.375" style="2" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="102.625" style="3" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="6.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="54.875" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -923,90 +1021,102 @@
       <c r="AH1" t="s">
         <v>76</v>
       </c>
+      <c r="AI1" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AJ1" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="AK1" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AL1" s="3" t="s">
+        <v>79</v>
+      </c>
     </row>
-    <row r="2" spans="1:34" ht="27" x14ac:dyDescent="0.15">
-      <c r="A2" t="s">
+    <row r="2" spans="1:38" s="8" customFormat="1" ht="101.25" x14ac:dyDescent="0.15">
+      <c r="A2" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="8" t="s">
         <v>34</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="L2" t="s">
+      <c r="L2" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="M2" t="s">
+      <c r="M2" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="N2" t="s">
+      <c r="N2" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="O2" t="s">
+      <c r="O2" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="P2" t="s">
+      <c r="P2" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="Q2" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="R2" t="s">
+      <c r="R2" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="S2" t="s">
+      <c r="S2" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="T2" t="s">
+      <c r="T2" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="U2" t="s">
+      <c r="U2" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="V2" t="s">
+      <c r="V2" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="W2" t="s">
+      <c r="W2" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="X2" t="s">
+      <c r="X2" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="Y2" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="Z2" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AA2" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AB2" s="8" t="s">
         <v>58</v>
       </c>
       <c r="AC2" s="1" t="s">
@@ -1021,14 +1131,21 @@
       <c r="AF2" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="AG2" t="s">
+      <c r="AG2" s="8" t="s">
         <v>59</v>
       </c>
       <c r="AH2" s="1" t="s">
         <v>77</v>
       </c>
+      <c r="AJ2" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="AK2" s="5"/>
+      <c r="AL2" s="6" t="s">
+        <v>84</v>
+      </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A3">
         <f>B3*100+C3</f>
         <v>100101</v>
@@ -1133,8 +1250,12 @@
       <c r="AH3" s="2" t="b">
         <v>1</v>
       </c>
+      <c r="AK3" s="3"/>
+      <c r="AL3" s="4" t="s">
+        <v>88</v>
+      </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A4" s="2">
         <f t="shared" ref="A4:A16" si="0">B4*100+C4</f>
         <v>100102</v>
@@ -1239,8 +1360,18 @@
       <c r="AH4" s="2" t="b">
         <v>1</v>
       </c>
+      <c r="AI4" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="AJ4" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="AK4" s="3"/>
+      <c r="AL4" s="4" t="s">
+        <v>88</v>
+      </c>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A5" s="2">
         <f t="shared" si="0"/>
         <v>100103</v>
@@ -1345,8 +1476,9 @@
       <c r="AH5" s="2" t="b">
         <v>1</v>
       </c>
+      <c r="AK5" s="3"/>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A6" s="2">
         <f t="shared" si="0"/>
         <v>100201</v>
@@ -1451,8 +1583,12 @@
       <c r="AH6" s="2" t="b">
         <v>1</v>
       </c>
+      <c r="AK6" s="3"/>
+      <c r="AL6" s="4" t="s">
+        <v>89</v>
+      </c>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A7" s="2">
         <f t="shared" si="0"/>
         <v>100202</v>
@@ -1557,8 +1693,9 @@
       <c r="AH7" s="2" t="b">
         <v>1</v>
       </c>
+      <c r="AK7" s="3"/>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A8" s="2">
         <f t="shared" si="0"/>
         <v>100301</v>
@@ -1663,8 +1800,18 @@
       <c r="AH8" s="2" t="b">
         <v>1</v>
       </c>
+      <c r="AI8" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="AJ8" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="AK8" s="3"/>
+      <c r="AL8" s="4" t="s">
+        <v>85</v>
+      </c>
     </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:38" x14ac:dyDescent="0.15">
       <c r="A9" s="2">
         <f t="shared" si="0"/>
         <v>100302</v>
@@ -1769,8 +1916,9 @@
       <c r="AH9" s="2" t="b">
         <v>1</v>
       </c>
+      <c r="AK9" s="3"/>
     </row>
-    <row r="10" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:38" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A10" s="2">
         <f t="shared" si="0"/>
         <v>900101</v>
@@ -1875,8 +2023,11 @@
       <c r="AH10" s="2" t="b">
         <v>1</v>
       </c>
+      <c r="AJ10" s="3"/>
+      <c r="AK10" s="3"/>
+      <c r="AL10" s="3"/>
     </row>
-    <row r="11" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:38" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A11" s="2">
         <f t="shared" si="0"/>
         <v>900102</v>
@@ -1981,8 +2132,11 @@
       <c r="AH11" s="2" t="b">
         <v>1</v>
       </c>
+      <c r="AJ11" s="3"/>
+      <c r="AK11" s="3"/>
+      <c r="AL11" s="3"/>
     </row>
-    <row r="12" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:38" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A12" s="2">
         <f t="shared" si="0"/>
         <v>900103</v>
@@ -2087,8 +2241,11 @@
       <c r="AH12" s="2" t="b">
         <v>1</v>
       </c>
+      <c r="AJ12" s="3"/>
+      <c r="AK12" s="3"/>
+      <c r="AL12" s="3"/>
     </row>
-    <row r="13" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:38" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A13" s="2">
         <f t="shared" si="0"/>
         <v>900201</v>
@@ -2193,8 +2350,11 @@
       <c r="AH13" s="2" t="b">
         <v>1</v>
       </c>
+      <c r="AJ13" s="3"/>
+      <c r="AK13" s="3"/>
+      <c r="AL13" s="3"/>
     </row>
-    <row r="14" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:38" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A14" s="2">
         <f t="shared" si="0"/>
         <v>900202</v>
@@ -2299,8 +2459,11 @@
       <c r="AH14" s="2" t="b">
         <v>1</v>
       </c>
+      <c r="AJ14" s="3"/>
+      <c r="AK14" s="3"/>
+      <c r="AL14" s="3"/>
     </row>
-    <row r="15" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:38" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A15" s="2">
         <f t="shared" si="0"/>
         <v>900301</v>
@@ -2405,8 +2568,11 @@
       <c r="AH15" s="2" t="b">
         <v>1</v>
       </c>
+      <c r="AJ15" s="3"/>
+      <c r="AK15" s="3"/>
+      <c r="AL15" s="3"/>
     </row>
-    <row r="16" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:38" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A16" s="2">
         <f t="shared" si="0"/>
         <v>900302</v>
@@ -2511,6 +2677,8 @@
       <c r="AH16" s="2" t="b">
         <v>1</v>
       </c>
+      <c r="AJ16" s="3"/>
+      <c r="AL16" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>